<commit_message>
updated code related to subObject impl
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/single/rules-that-return-single-item-with-subObject.drl.xlsx
+++ b/src/main/resources/rules/single/rules-that-return-single-item-with-subObject.drl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abijit/Projects/droolspoc/src/main/resources/rules/single/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D04D3D-2599-3B4E-96EB-B50E58AF304C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEDDEFD-5F97-7D4E-A279-9E383589910E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>RuleSet</t>
   </si>
@@ -86,15 +86,6 @@
   </si>
   <si>
     <t>Response - Value</t>
-  </si>
-  <si>
-    <t>Response - SubResponse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">		logger.info("response before setting subResponse: {}", response);
-		logger.info("output value: {}", $1);
-		response.setSubResponse($1);
-		logger.info("response after setting subResponse: {}", response);</t>
   </si>
   <si>
     <t>response:Response()
@@ -112,6 +103,35 @@
   <si>
     <t>logger.info("Response - value: {}", $1);
 		response.setValue($1);</t>
+  </si>
+  <si>
+    <t>SubResponse - subValue</t>
+  </si>
+  <si>
+    <t>SubResponse - Text</t>
+  </si>
+  <si>
+    <t>"sub text 1"</t>
+  </si>
+  <si>
+    <t>"sub text 2"</t>
+  </si>
+  <si>
+    <t>"sub text 3"</t>
+  </si>
+  <si>
+    <t>"sub text 4"</t>
+  </si>
+  <si>
+    <t>SubResponse subResponse = new SubResponse();
+		subResponse.setSubValue($1);</t>
+  </si>
+  <si>
+    <t>subResponse.setText($1);
+		logger.info("response before setting subResponse: {}", response);
+		logger.info("subResponse: {}", subResponse);
+		response.setSubResponse(subResponse);		
+		logger.info("response after setting subResponse: {}", response);</t>
   </si>
 </sst>
 </file>
@@ -227,7 +247,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -235,9 +255,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -262,6 +279,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -269,12 +292,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -591,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -602,200 +619,228 @@
     <col min="1" max="1" width="31.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="61" style="1" customWidth="1"/>
+    <col min="4" max="5" width="50.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="61.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A1" s="5"/>
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A1" s="4"/>
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="5"/>
-      <c r="B2" s="9" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="4"/>
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="5"/>
-      <c r="B3" s="9" t="s">
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="4"/>
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="5"/>
-      <c r="B4" s="9" t="s">
+      <c r="C3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="4"/>
+      <c r="B4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="11" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="9"/>
-      <c r="B8" s="13" t="s">
+      <c r="F7" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="8"/>
+      <c r="B8" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.15">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.15">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="E9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.15">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>1</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>5</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A12" s="7" t="s">
+      <c r="F11" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.15">
+      <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>2</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>3</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="6" t="s">
+      <c r="F12" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>3</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>2</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="6" t="s">
+      <c r="F13" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>4</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>10</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>4</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C2:F2"/>
     <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39409448818897608" bottom="0.39409448818897608" header="0" footer="0"/>

</xml_diff>